<commit_message>
Modify Millenium-LawOfRiver tab to explicitly represent Upper Basin curtailment
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F219F5C1-0A48-4EBA-812D-88A53ABC946C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE54361-76BA-462E-BE60-D4A4037A86AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -573,9 +573,6 @@
     <t>Mellennium-LawOfRiver</t>
   </si>
   <si>
-    <t xml:space="preserve">A completed role play of the Millennium Droughtfor 10 more years where political decisions follow the existing Law of the River and Lower Basin Drought Contingency Plan </t>
-  </si>
-  <si>
     <t>Players enter their release from Lake Mead in cells C82 to C85. Users must specify an additional release to cover downstream evaporation from Lake Mohave and Havasu plus riparian evapotranspiration. A lookup table is provided in Cells O82 to S91 should players want to cutback releases according to the current Lower Basin Drought Contingency Plan.</t>
   </si>
   <si>
@@ -595,6 +592,9 @@
   </si>
   <si>
     <t>DIRECTIONS TO ROLE PLAY:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A completed role play of the Millennium Droughtfor 10 more years where political decisions follow the Law of the River Articles 3a (7.5/7.5 split), 3d (Upper basin curtailment),  and Lower Basin Drought Contingency Plan </t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -951,11 +951,23 @@
     <xf numFmtId="167" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -969,25 +981,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18692,8 +18695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18712,20 +18715,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
+      <c r="A1" s="53" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -18742,36 +18745,36 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="58" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+    </row>
+    <row r="5" spans="1:12" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="58" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-    </row>
-    <row r="5" spans="1:12" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="16"/>
@@ -18787,92 +18790,92 @@
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="58"/>
+      <c r="A7" s="60" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="62"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>1</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>2</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="55"/>
     </row>
     <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>3</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>4</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="55"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="52" t="s">
@@ -18894,91 +18897,91 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="55"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
     </row>
     <row r="15" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="54" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="55"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="55"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="55"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
@@ -19000,163 +19003,163 @@
       <c r="A19" s="29">
         <v>10</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="55"/>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
         <v>11</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="55"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29">
         <v>12</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="55"/>
     </row>
     <row r="22" spans="1:12" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
         <v>13</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="55"/>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
         <v>14</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="60"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
         <v>15</v>
       </c>
-      <c r="B24" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="54"/>
+      <c r="B24" s="54" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="55"/>
     </row>
     <row r="25" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29">
         <v>16</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="55"/>
     </row>
     <row r="26" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
         <v>17</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="55"/>
     </row>
     <row r="27" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="29">
         <v>18</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="55"/>
     </row>
     <row r="28" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="52" t="s">
@@ -19178,55 +19181,55 @@
       <c r="A29" s="29">
         <v>19</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
     </row>
     <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29">
         <v>20</v>
       </c>
-      <c r="B30" s="59" t="s">
+      <c r="B30" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="60"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="57"/>
     </row>
     <row r="31" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
         <v>21</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="62"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="64"/>
     </row>
     <row r="32" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
@@ -19267,7 +19270,7 @@
         <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
@@ -19275,7 +19278,7 @@
         <v>179</v>
       </c>
       <c r="C37" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
@@ -19303,33 +19306,23 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="55" t="s">
-        <v>184</v>
-      </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="55"/>
-      <c r="F42" s="55"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="55"/>
+      <c r="A42" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A5:L5"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
@@ -19346,6 +19339,16 @@
     <mergeCell ref="B19:L19"/>
     <mergeCell ref="B20:L20"/>
     <mergeCell ref="B21:L21"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19378,7 +19381,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -23456,7 +23459,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -26430,7 +26433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551E70D5-97BA-4F5D-AF13-D96C10A68BB9}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -26452,7 +26457,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -26710,7 +26715,7 @@
       </c>
       <c r="D24" s="15">
         <f>IF(D$23&lt;&gt;"",C54,"")</f>
-        <v>10.627103119999429</v>
+        <v>10.627103119999427</v>
       </c>
       <c r="E24" s="15">
         <f t="shared" ref="E24:L24" si="1">IF(E$23&lt;&gt;"",D54,"")</f>
@@ -26718,7 +26723,7 @@
       </c>
       <c r="F24" s="15">
         <f t="shared" si="1"/>
-        <v>9.9147267200005764</v>
+        <v>9.9147267200005746</v>
       </c>
       <c r="G24" s="15">
         <f t="shared" si="1"/>
@@ -26726,11 +26731,11 @@
       </c>
       <c r="H24" s="15">
         <f t="shared" si="1"/>
-        <v>9.2468580950000039</v>
+        <v>9.2468580950000021</v>
       </c>
       <c r="I24" s="15">
         <f t="shared" si="1"/>
-        <v>8.9295740165000037</v>
+        <v>8.9295740165000019</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="1"/>
@@ -26758,39 +26763,39 @@
       </c>
       <c r="D25" s="15">
         <f>IF(D$23&lt;&gt;"",C51,"")</f>
-        <v>10.554603119999427</v>
+        <v>10.627103119999427</v>
       </c>
       <c r="E25" s="15">
         <f t="shared" ref="E25:L27" si="2">IF(E$23&lt;&gt;"",D51,"")</f>
-        <v>10.123836663056064</v>
+        <v>10.265345360000001</v>
       </c>
       <c r="F25" s="15">
         <f t="shared" si="2"/>
-        <v>9.7076190954441497</v>
+        <v>9.9147267200005746</v>
       </c>
       <c r="G25" s="15">
         <f t="shared" si="2"/>
-        <v>9.3058594899772444</v>
+        <v>9.5752423295005755</v>
       </c>
       <c r="H25" s="15">
         <f t="shared" si="2"/>
-        <v>8.9184337663987332</v>
+        <v>9.2468580950000021</v>
       </c>
       <c r="I25" s="15">
         <f t="shared" si="2"/>
-        <v>8.5452464019577921</v>
+        <v>8.9295740165000019</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="2"/>
-        <v>8.186196571565441</v>
+        <v>8.6233900939994292</v>
       </c>
       <c r="K25" s="15">
         <f t="shared" si="2"/>
-        <v>7.8411779143244686</v>
+        <v>8.3283063274994298</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="2"/>
-        <v>7.5087719436694496</v>
+        <v>8.0429351975000039</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -26806,39 +26811,39 @@
       </c>
       <c r="D26" s="15">
         <f>IF(D$23&lt;&gt;"",C52,"")</f>
-        <v>7.2500000000000675E-2</v>
+        <v>0</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" si="2"/>
-        <v>0.1415086969439372</v>
+        <v>0</v>
       </c>
       <c r="F26" s="15">
         <f t="shared" si="2"/>
-        <v>0.20710762455642673</v>
+        <v>0</v>
       </c>
       <c r="G26" s="15">
         <f t="shared" si="2"/>
-        <v>0.26938283952333109</v>
+        <v>0</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" si="2"/>
-        <v>0.32842432860127158</v>
+        <v>0</v>
       </c>
       <c r="I26" s="15">
         <f t="shared" si="2"/>
-        <v>0.38432761454221165</v>
+        <v>0</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="2"/>
-        <v>0.43719352243398912</v>
+        <v>0</v>
       </c>
       <c r="K26" s="15">
         <f t="shared" si="2"/>
-        <v>0.48712841317496114</v>
+        <v>0</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="2"/>
-        <v>0.5341632538305543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -26946,39 +26951,39 @@
       </c>
       <c r="D29" s="15">
         <f t="shared" ref="D29:L29" si="3">IF(D$23&lt;&gt;"",D$28*D25/SUM(D$25:D$27),"")</f>
-        <v>0.50826645694336314</v>
+        <v>0.51175775999942696</v>
       </c>
       <c r="E29" s="15">
         <f t="shared" si="3"/>
-        <v>0.49371756761191554</v>
+        <v>0.50061863999942702</v>
       </c>
       <c r="F29" s="15">
         <f t="shared" si="3"/>
-        <v>0.47925960546690344</v>
+        <v>0.48948439050000009</v>
       </c>
       <c r="G29" s="15">
         <f t="shared" si="3"/>
-        <v>0.46492572357851253</v>
+        <v>0.47838423450057299</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="3"/>
-        <v>0.45068736444093926</v>
+        <v>0.46728407849999998</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="3"/>
-        <v>0.43654983039235018</v>
+        <v>0.45618392250057305</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="3"/>
-        <v>0.42251865724097143</v>
+        <v>0.44508376650000003</v>
       </c>
       <c r="K29" s="15">
         <f t="shared" si="3"/>
-        <v>0.40990597065501944</v>
+        <v>0.43537112999942701</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="3"/>
-        <v>0.39706812384103285</v>
+        <v>0.42531498000000006</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -26992,39 +26997,39 @@
       </c>
       <c r="D30" s="15">
         <f t="shared" si="4"/>
-        <v>3.4913030560637672E-3</v>
+        <v>0</v>
       </c>
       <c r="E30" s="15">
         <f t="shared" si="4"/>
-        <v>6.9010723875114616E-3</v>
+        <v>0</v>
       </c>
       <c r="F30" s="15">
         <f t="shared" si="4"/>
-        <v>1.0224785033096656E-2</v>
+        <v>0</v>
       </c>
       <c r="G30" s="15">
         <f t="shared" si="4"/>
-        <v>1.3458510922060492E-2</v>
+        <v>0</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="4"/>
-        <v>1.6596714059060762E-2</v>
+        <v>0</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="4"/>
-        <v>1.9634092108222832E-2</v>
+        <v>0</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="4"/>
-        <v>2.2565109259028611E-2</v>
+        <v>0</v>
       </c>
       <c r="K30" s="15">
         <f t="shared" si="4"/>
-        <v>2.5465159344407549E-2</v>
+        <v>0</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="4"/>
-        <v>2.8246856158967215E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -27168,97 +27173,94 @@
       <c r="A34" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="24">
-        <v>0.35</v>
-      </c>
+      <c r="B34" s="24"/>
       <c r="C34" s="15">
-        <f>IF(C$23&lt;&gt;"",C$33*$B34,"")</f>
-        <v>4.0774999999999997</v>
+        <f>IF(C$23&lt;&gt;"",IF(C33&lt;$B35,0,C33-$B35),"")</f>
+        <v>4.1500000000000004</v>
       </c>
       <c r="D34" s="15">
-        <f t="shared" ref="D34:L35" si="7">IF(D$23&lt;&gt;"",D$33*$B34,"")</f>
-        <v>4.0774999999999997</v>
+        <f t="shared" ref="D34:L34" si="7">IF(D$23&lt;&gt;"",IF(D33&lt;$B35,0,D33-$B35),"")</f>
+        <v>4.1500000000000004</v>
       </c>
       <c r="E34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="F34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="G34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="H34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="K34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" si="7"/>
-        <v>4.0774999999999997</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="24">
-        <f>1-B34</f>
-        <v>0.65</v>
+      <c r="B35" s="66">
+        <v>7.5</v>
       </c>
       <c r="C35" s="15">
-        <f>IF(C$23&lt;&gt;"",C$33*$B35,"")</f>
-        <v>7.5725000000000007</v>
+        <f>IF(C23&lt;&gt;"",IF(C33&lt;$B35,C33,$B35),"")</f>
+        <v>7.5</v>
       </c>
       <c r="D35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" ref="D35:L35" si="8">IF(D23&lt;&gt;"",IF(D33&lt;$B35,D33,$B35),"")</f>
+        <v>7.5</v>
       </c>
       <c r="E35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="F35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="G35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="H35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="I35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="J35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="K35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
       <c r="L35" s="15">
-        <f t="shared" si="7"/>
-        <v>7.5725000000000007</v>
+        <f t="shared" si="8"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
@@ -27353,43 +27355,43 @@
       </c>
       <c r="C42" s="15">
         <f>IF(C$23&lt;&gt;"",C25+C34-C29-C37,"")</f>
-        <v>14.554603119999427</v>
+        <v>14.627103119999427</v>
       </c>
       <c r="D42" s="15">
-        <f t="shared" ref="D42:L42" si="8">IF(D$23&lt;&gt;"",D25+D34-D29-D37,"")</f>
-        <v>14.123836663056064</v>
+        <f t="shared" ref="D42:L42" si="9">IF(D$23&lt;&gt;"",D25+D34-D29-D37,"")</f>
+        <v>14.265345360000001</v>
       </c>
       <c r="E42" s="15">
-        <f t="shared" si="8"/>
-        <v>13.70761909544415</v>
+        <f t="shared" si="9"/>
+        <v>13.914726720000575</v>
       </c>
       <c r="F42" s="15">
-        <f t="shared" si="8"/>
-        <v>13.305859489977244</v>
+        <f t="shared" si="9"/>
+        <v>13.575242329500576</v>
       </c>
       <c r="G42" s="15">
-        <f t="shared" si="8"/>
-        <v>12.918433766398733</v>
+        <f t="shared" si="9"/>
+        <v>13.246858095000002</v>
       </c>
       <c r="H42" s="15">
-        <f t="shared" si="8"/>
-        <v>12.545246401957792</v>
+        <f t="shared" si="9"/>
+        <v>12.929574016500002</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="8"/>
-        <v>12.186196571565441</v>
+        <f t="shared" si="9"/>
+        <v>12.623390093999429</v>
       </c>
       <c r="J42" s="15">
-        <f t="shared" si="8"/>
-        <v>11.841177914324469</v>
+        <f t="shared" si="9"/>
+        <v>12.32830632749943</v>
       </c>
       <c r="K42" s="15">
-        <f t="shared" si="8"/>
-        <v>11.50877194366945</v>
+        <f t="shared" si="9"/>
+        <v>12.042935197500004</v>
       </c>
       <c r="L42" s="15">
-        <f t="shared" si="8"/>
-        <v>11.189203819828416</v>
+        <f t="shared" si="9"/>
+        <v>11.767620217500005</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
@@ -27398,43 +27400,43 @@
       </c>
       <c r="C43" s="15">
         <f>IF(C$23&lt;&gt;"",C26+C35-C30+C37+C39,"")</f>
-        <v>7.5725000000000007</v>
+        <v>7.5</v>
       </c>
       <c r="D43" s="15">
-        <f t="shared" ref="D43:L43" si="9">IF(D$23&lt;&gt;"",D26+D35-D30+D37+D39,"")</f>
-        <v>7.6415086969439372</v>
+        <f t="shared" ref="D43:L43" si="10">IF(D$23&lt;&gt;"",D26+D35-D30+D37+D39,"")</f>
+        <v>7.5</v>
       </c>
       <c r="E43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.7071076245564267</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="F43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.7693828395233311</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="G43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.8284243286012716</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="H43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.8843276145422116</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="I43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.9371935224339891</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="J43" s="15">
-        <f t="shared" si="9"/>
-        <v>7.9871284131749611</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="K43" s="15">
-        <f t="shared" si="9"/>
-        <v>8.0341632538305543</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="L43" s="15">
-        <f t="shared" si="9"/>
-        <v>8.078416397671587</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
@@ -27446,39 +27448,39 @@
         <v>0.75</v>
       </c>
       <c r="D44" s="26">
-        <f t="shared" ref="D44:L44" si="10">IF(D$23&lt;&gt;"",D27+D32-D31-D39,"")</f>
+        <f t="shared" ref="D44:L44" si="11">IF(D$23&lt;&gt;"",D27+D32-D31-D39,"")</f>
         <v>0.75</v>
       </c>
       <c r="E44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="F44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="G44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="H44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="I44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="J44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="K44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
       <c r="L44" s="26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.75</v>
       </c>
     </row>
@@ -27510,35 +27512,35 @@
         <v>4</v>
       </c>
       <c r="E46" s="25">
-        <f t="shared" ref="E46:L48" si="11">D46</f>
+        <f t="shared" ref="E46:L48" si="12">D46</f>
         <v>4</v>
       </c>
       <c r="F46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="G46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="I46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="J46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="L46" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
     </row>
@@ -27550,39 +27552,39 @@
         <v>7.5</v>
       </c>
       <c r="D47" s="25">
-        <f t="shared" ref="D47:G48" si="12">C47</f>
+        <f t="shared" ref="D47:G48" si="13">C47</f>
         <v>7.5</v>
       </c>
       <c r="E47" s="25">
+        <f t="shared" si="13"/>
+        <v>7.5</v>
+      </c>
+      <c r="F47" s="25">
+        <f t="shared" si="13"/>
+        <v>7.5</v>
+      </c>
+      <c r="G47" s="25">
+        <f t="shared" si="13"/>
+        <v>7.5</v>
+      </c>
+      <c r="H47" s="25">
         <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
-      <c r="F47" s="25">
+      <c r="I47" s="25">
         <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
-      <c r="G47" s="25">
+      <c r="J47" s="25">
         <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
-      <c r="H47" s="25">
-        <f t="shared" si="11"/>
+      <c r="K47" s="25">
+        <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
-      <c r="I47" s="25">
-        <f t="shared" si="11"/>
-        <v>7.5</v>
-      </c>
-      <c r="J47" s="25">
-        <f t="shared" si="11"/>
-        <v>7.5</v>
-      </c>
-      <c r="K47" s="25">
-        <f t="shared" si="11"/>
-        <v>7.5</v>
-      </c>
       <c r="L47" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.5</v>
       </c>
     </row>
@@ -27594,39 +27596,39 @@
         <v>0.75</v>
       </c>
       <c r="D48" s="25">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="E48" s="25">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="F48" s="25">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="G48" s="25">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="H48" s="25">
         <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-      <c r="E48" s="25">
+      <c r="I48" s="25">
         <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-      <c r="F48" s="25">
+      <c r="J48" s="25">
         <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-      <c r="G48" s="25">
+      <c r="K48" s="25">
         <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-      <c r="H48" s="25">
-        <f t="shared" si="11"/>
-        <v>0.75</v>
-      </c>
-      <c r="I48" s="25">
-        <f t="shared" si="11"/>
-        <v>0.75</v>
-      </c>
-      <c r="J48" s="25">
-        <f t="shared" si="11"/>
-        <v>0.75</v>
-      </c>
-      <c r="K48" s="25">
-        <f t="shared" si="11"/>
-        <v>0.75</v>
-      </c>
       <c r="L48" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
     </row>
@@ -27644,35 +27646,35 @@
         <v>8.25</v>
       </c>
       <c r="E49" s="15">
-        <f t="shared" ref="E49:L49" si="13">IF(E$23&lt;&gt;"",SUM(E47:E48),"")</f>
+        <f t="shared" ref="E49:L49" si="14">IF(E$23&lt;&gt;"",SUM(E47:E48),"")</f>
         <v>8.25</v>
       </c>
       <c r="F49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="G49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="H49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="J49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="K49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
       <c r="L49" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8.25</v>
       </c>
     </row>
@@ -27697,43 +27699,43 @@
       </c>
       <c r="C51" s="15">
         <f>IF(C$23&lt;&gt;"",C42-C46,"")</f>
-        <v>10.554603119999427</v>
+        <v>10.627103119999427</v>
       </c>
       <c r="D51" s="15">
         <f>IF(D$23&lt;&gt;"",D42-D46,"")</f>
-        <v>10.123836663056064</v>
+        <v>10.265345360000001</v>
       </c>
       <c r="E51" s="15">
-        <f t="shared" ref="E51:L53" si="14">IF(E$23&lt;&gt;"",E42-E46,"")</f>
-        <v>9.7076190954441497</v>
+        <f t="shared" ref="E51:L53" si="15">IF(E$23&lt;&gt;"",E42-E46,"")</f>
+        <v>9.9147267200005746</v>
       </c>
       <c r="F51" s="15">
-        <f t="shared" si="14"/>
-        <v>9.3058594899772444</v>
+        <f t="shared" si="15"/>
+        <v>9.5752423295005755</v>
       </c>
       <c r="G51" s="15">
-        <f t="shared" si="14"/>
-        <v>8.9184337663987332</v>
+        <f t="shared" si="15"/>
+        <v>9.2468580950000021</v>
       </c>
       <c r="H51" s="15">
-        <f t="shared" si="14"/>
-        <v>8.5452464019577921</v>
+        <f t="shared" si="15"/>
+        <v>8.9295740165000019</v>
       </c>
       <c r="I51" s="15">
-        <f t="shared" si="14"/>
-        <v>8.186196571565441</v>
+        <f t="shared" si="15"/>
+        <v>8.6233900939994292</v>
       </c>
       <c r="J51" s="15">
-        <f t="shared" si="14"/>
-        <v>7.8411779143244686</v>
+        <f t="shared" si="15"/>
+        <v>8.3283063274994298</v>
       </c>
       <c r="K51" s="15">
-        <f t="shared" si="14"/>
-        <v>7.5087719436694496</v>
+        <f t="shared" si="15"/>
+        <v>8.0429351975000039</v>
       </c>
       <c r="L51" s="15">
-        <f t="shared" si="14"/>
-        <v>7.1892038198284158</v>
+        <f t="shared" si="15"/>
+        <v>7.7676202175000046</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
@@ -27741,44 +27743,44 @@
         <v>5</v>
       </c>
       <c r="C52" s="15">
-        <f t="shared" ref="C52:D53" si="15">IF(C$23&lt;&gt;"",C43-C47,"")</f>
-        <v>7.2500000000000675E-2</v>
+        <f t="shared" ref="C52:D53" si="16">IF(C$23&lt;&gt;"",C43-C47,"")</f>
+        <v>0</v>
       </c>
       <c r="D52" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="15">
         <f t="shared" si="15"/>
-        <v>0.1415086969439372</v>
-      </c>
-      <c r="E52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.20710762455642673</v>
+        <v>0</v>
       </c>
       <c r="F52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.26938283952333109</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="G52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.32842432860127158</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="H52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.38432761454221165</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="I52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.43719352243398912</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="J52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.48712841317496114</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="K52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.5341632538305543</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
       <c r="L52" s="15">
-        <f t="shared" si="14"/>
-        <v>0.57841639767158703</v>
+        <f t="shared" si="15"/>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
@@ -27786,43 +27788,43 @@
         <v>6</v>
       </c>
       <c r="C53" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="15">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="D53" s="15">
+      <c r="F53" s="15">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="E53" s="15">
-        <f t="shared" si="14"/>
+      <c r="G53" s="15">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="F53" s="15">
-        <f t="shared" si="14"/>
+      <c r="H53" s="15">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G53" s="15">
-        <f t="shared" si="14"/>
+      <c r="I53" s="15">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="H53" s="15">
-        <f t="shared" si="14"/>
+      <c r="J53" s="15">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="I53" s="15">
-        <f t="shared" si="14"/>
+      <c r="K53" s="15">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J53" s="15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="K53" s="15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
       <c r="L53" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -27833,43 +27835,43 @@
       <c r="B54" s="1"/>
       <c r="C54" s="15">
         <f>IF(C$23&lt;&gt;"",SUM(C51:C53),"")</f>
-        <v>10.627103119999429</v>
+        <v>10.627103119999427</v>
       </c>
       <c r="D54" s="15">
         <f>IF(D$23&lt;&gt;"",SUM(D51:D53),"")</f>
         <v>10.265345360000001</v>
       </c>
       <c r="E54" s="15">
-        <f t="shared" ref="E54:L54" si="16">IF(E$23&lt;&gt;"",SUM(E51:E53),"")</f>
-        <v>9.9147267200005764</v>
+        <f t="shared" ref="E54:L54" si="17">IF(E$23&lt;&gt;"",SUM(E51:E53),"")</f>
+        <v>9.9147267200005746</v>
       </c>
       <c r="F54" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.5752423295005755</v>
       </c>
       <c r="G54" s="15">
-        <f t="shared" si="16"/>
-        <v>9.2468580950000039</v>
+        <f t="shared" si="17"/>
+        <v>9.2468580950000021</v>
       </c>
       <c r="H54" s="15">
-        <f t="shared" si="16"/>
-        <v>8.9295740165000037</v>
+        <f t="shared" si="17"/>
+        <v>8.9295740165000019</v>
       </c>
       <c r="I54" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.6233900939994292</v>
       </c>
       <c r="J54" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.3283063274994298</v>
       </c>
       <c r="K54" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.0429351975000039</v>
       </c>
       <c r="L54" s="15">
-        <f t="shared" si="16"/>
-        <v>7.7676202175000029</v>
+        <f t="shared" si="17"/>
+        <v>7.7676202175000046</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -27970,39 +27972,39 @@
         <v>0.8</v>
       </c>
       <c r="D62" s="12">
-        <f t="shared" ref="D62:L62" si="17">IF(D$23&lt;&gt;"",0.8,"")</f>
+        <f t="shared" ref="D62:L62" si="18">IF(D$23&lt;&gt;"",0.8,"")</f>
         <v>0.8</v>
       </c>
       <c r="E62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="F62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="G62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="H62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="I62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="J62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="K62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
       <c r="L62" s="12">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.8</v>
       </c>
     </row>
@@ -28018,39 +28020,39 @@
         <v>0.8</v>
       </c>
       <c r="D63" s="15">
-        <f t="shared" ref="D63:L64" si="18">IF(D$23&lt;&gt;"",D$62*$B63,"")</f>
+        <f t="shared" ref="D63:L64" si="19">IF(D$23&lt;&gt;"",D$62*$B63,"")</f>
         <v>0.8</v>
       </c>
       <c r="E63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="F63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="G63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="H63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="I63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="J63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="K63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
       <c r="L63" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.8</v>
       </c>
     </row>
@@ -28067,39 +28069,39 @@
         <v>0</v>
       </c>
       <c r="D64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="J64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="K64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L64" s="15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -28112,39 +28114,39 @@
         <v>9.0500000000000007</v>
       </c>
       <c r="D65" s="15">
-        <f t="shared" ref="D65:L65" si="19">IF(D$23&lt;&gt;"",D62+D49,"")</f>
+        <f t="shared" ref="D65:L65" si="20">IF(D$23&lt;&gt;"",D62+D49,"")</f>
         <v>9.0500000000000007</v>
       </c>
       <c r="E65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="F65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="G65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="H65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="I65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="J65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="K65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
       <c r="L65" s="15">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.0500000000000007</v>
       </c>
     </row>
@@ -28161,35 +28163,35 @@
         <v>0.75</v>
       </c>
       <c r="E66" s="25">
-        <f t="shared" ref="E66:L66" si="20">D66</f>
+        <f t="shared" ref="E66:L66" si="21">D66</f>
         <v>0.75</v>
       </c>
       <c r="F66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="G66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="H66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="I66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="J66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="K66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
       <c r="L66" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.75</v>
       </c>
     </row>
@@ -28207,35 +28209,35 @@
         <v>9.7228600849999989</v>
       </c>
       <c r="E67" s="15">
-        <f t="shared" ref="E67:L67" si="21">IF(E$23&lt;&gt;"",D90,"")</f>
+        <f t="shared" ref="E67:L67" si="22">IF(E$23&lt;&gt;"",D90,"")</f>
         <v>9.321006484999403</v>
       </c>
       <c r="F67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.0122623349994058</v>
       </c>
       <c r="G67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8.7119076850000035</v>
       </c>
       <c r="H67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8.4201686349994098</v>
       </c>
       <c r="I67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8.1370451849994119</v>
       </c>
       <c r="J67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.8614603849994147</v>
       </c>
       <c r="K67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.5944911849994163</v>
       </c>
       <c r="L67" s="15">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>7.5848642849994174</v>
       </c>
     </row>
@@ -28255,35 +28257,35 @@
         <v>9.7228600849999989</v>
       </c>
       <c r="E68" s="15">
-        <f t="shared" ref="E68:L69" si="22">IF(E$23&lt;&gt;"",D88,"")</f>
+        <f t="shared" ref="E68:L69" si="23">IF(E$23&lt;&gt;"",D88,"")</f>
         <v>9.321006484999403</v>
       </c>
       <c r="F68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9.0122623349994058</v>
       </c>
       <c r="G68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8.7119076850000035</v>
       </c>
       <c r="H68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8.4201686349994098</v>
       </c>
       <c r="I68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8.1370451849994119</v>
       </c>
       <c r="J68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.8614603849994147</v>
       </c>
       <c r="K68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.5944911849994163</v>
       </c>
       <c r="L68" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7.5848642849994174</v>
       </c>
     </row>
@@ -28303,35 +28305,35 @@
         <v>0</v>
       </c>
       <c r="E69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="I69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="K69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L69" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -28391,39 +28393,39 @@
         <v>0.49578791500000002</v>
       </c>
       <c r="D71" s="15">
-        <f t="shared" ref="D71:L72" si="23">IF(D$23&lt;&gt;"",D$70*D68/SUM(D$68:D$69),"")</f>
+        <f t="shared" ref="D71:L72" si="24">IF(D$23&lt;&gt;"",D$70*D68/SUM(D$68:D$69),"")</f>
         <v>0.48485360000059508</v>
       </c>
       <c r="E71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.47574415000000009</v>
       </c>
       <c r="F71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.46735464999940507</v>
       </c>
       <c r="G71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.45873905000059506</v>
       </c>
       <c r="H71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.45012345000000004</v>
       </c>
       <c r="I71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.4425848</v>
       </c>
       <c r="J71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.43396919999999994</v>
       </c>
       <c r="K71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.42662690000000003</v>
       </c>
       <c r="L71" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.42662690000000003</v>
       </c>
     </row>
@@ -28437,39 +28439,39 @@
         <v>0</v>
       </c>
       <c r="D72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="E72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="F72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L72" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -28493,35 +28495,35 @@
         <v>7.0651463999994055</v>
       </c>
       <c r="E74" s="15">
-        <f t="shared" ref="E74:L74" si="24">IF(E$23&lt;&gt;"",E47+E63-E71-E66,"")</f>
+        <f t="shared" ref="E74:L74" si="25">IF(E$23&lt;&gt;"",E47+E63-E71-E66,"")</f>
         <v>7.074255850000001</v>
       </c>
       <c r="F74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.0826453500005959</v>
       </c>
       <c r="G74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.0912609499994055</v>
       </c>
       <c r="H74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.0998765500000003</v>
       </c>
       <c r="I74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.107415200000001</v>
       </c>
       <c r="J74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.1160308000000008</v>
       </c>
       <c r="K74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.1233731000000002</v>
       </c>
       <c r="L74" s="15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.1233731000000002</v>
       </c>
     </row>
@@ -28534,39 +28536,39 @@
         <v>1.5</v>
       </c>
       <c r="D75" s="15">
-        <f t="shared" ref="D75:L75" si="25">IF(D$23&lt;&gt;"",D48+D64-D72+D66,"")</f>
+        <f t="shared" ref="D75:L75" si="26">IF(D$23&lt;&gt;"",D48+D64-D72+D66,"")</f>
         <v>1.5</v>
       </c>
       <c r="E75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="F75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="G75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="H75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="I75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="J75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="K75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
       <c r="L75" s="15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.5</v>
       </c>
     </row>
@@ -28603,39 +28605,39 @@
         <v>0</v>
       </c>
       <c r="D78" s="32">
-        <f t="shared" ref="D78:L78" si="26">IF(D23&lt;&gt;"",300*D77,"")</f>
+        <f t="shared" ref="D78:L78" si="27">IF(D23&lt;&gt;"",300*D77,"")</f>
         <v>0</v>
       </c>
       <c r="E78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="H78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L78" s="32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M78" s="34">
@@ -28659,39 +28661,39 @@
         <v>17.189860084999999</v>
       </c>
       <c r="D80" s="15">
-        <f t="shared" ref="D80:L80" si="27">IF(D$23&lt;&gt;"",D68+D74+D77,"")</f>
+        <f t="shared" ref="D80:L80" si="28">IF(D$23&lt;&gt;"",D68+D74+D77,"")</f>
         <v>16.788006484999404</v>
       </c>
       <c r="E80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>16.395262334999405</v>
       </c>
       <c r="F80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>16.094907685000003</v>
       </c>
       <c r="G80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>15.803168634999409</v>
       </c>
       <c r="H80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>15.520045184999411</v>
       </c>
       <c r="I80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>15.244460384999414</v>
       </c>
       <c r="J80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>14.977491184999415</v>
       </c>
       <c r="K80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>14.717864284999417</v>
       </c>
       <c r="L80" s="15">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>14.708237384999418</v>
       </c>
     </row>
@@ -28704,39 +28706,39 @@
         <v>1.5</v>
       </c>
       <c r="D81" s="15">
-        <f t="shared" ref="D81:L81" si="28">IF(D$23&lt;&gt;"",D69+D75-D77,"")</f>
+        <f t="shared" ref="D81:L81" si="29">IF(D$23&lt;&gt;"",D69+D75-D77,"")</f>
         <v>1.5</v>
       </c>
       <c r="E81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="F81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="G81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="H81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="I81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="J81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="K81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
       <c r="L81" s="15">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.5</v>
       </c>
     </row>
@@ -28768,39 +28770,39 @@
         <v>6.867</v>
       </c>
       <c r="D83" s="50">
-        <f t="shared" ref="D83:L83" si="29">IF(D23&lt;&gt;"",7.5-VLOOKUP(D67,$P$84:$S$91,2),"")</f>
+        <f t="shared" ref="D83:L83" si="30">IF(D23&lt;&gt;"",7.5-VLOOKUP(D67,$P$84:$S$91,2),"")</f>
         <v>6.867</v>
       </c>
       <c r="E83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="F83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="G83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="H83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="I83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="J83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.7829999999999995</v>
       </c>
       <c r="K83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.5330000000000004</v>
       </c>
       <c r="L83" s="50">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>6.5330000000000004</v>
       </c>
       <c r="O83" s="46" t="s">
@@ -28832,35 +28834,35 @@
         <v>0.6</v>
       </c>
       <c r="E84" s="12">
-        <f t="shared" ref="E84:L84" si="30">IF(E$23&lt;&gt;"",D84,"")</f>
+        <f t="shared" ref="E84:L84" si="31">IF(E$23&lt;&gt;"",D84,"")</f>
         <v>0.6</v>
       </c>
       <c r="F84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="H84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="I84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="J84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="K84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="L84" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="O84" s="44">
@@ -28871,7 +28873,7 @@
         <v>5.981122</v>
       </c>
       <c r="Q84" s="47">
-        <f t="shared" ref="Q84:Q91" si="31">S84-R84</f>
+        <f t="shared" ref="Q84:Q91" si="32">S84-R84</f>
         <v>1.2</v>
       </c>
       <c r="R84" s="43">
@@ -28893,35 +28895,35 @@
         <v>1.5</v>
       </c>
       <c r="E85" s="25">
-        <f t="shared" ref="E85:L85" si="32">D85</f>
+        <f t="shared" ref="E85:L85" si="33">D85</f>
         <v>1.5</v>
       </c>
       <c r="F85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="G85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="H85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="I85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="J85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="K85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="L85" s="25">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.5</v>
       </c>
       <c r="O85" s="44">
@@ -28932,7 +28934,7 @@
         <v>6.305377</v>
       </c>
       <c r="Q85" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1.117</v>
       </c>
       <c r="R85" s="43">
@@ -28952,39 +28954,39 @@
         <v>8.9669999999999987</v>
       </c>
       <c r="D86" s="15">
-        <f t="shared" ref="D86:L86" si="33">IF(D$23&lt;&gt;"",SUM(D83:D85),"")</f>
+        <f t="shared" ref="D86:L86" si="34">IF(D$23&lt;&gt;"",SUM(D83:D85),"")</f>
         <v>8.9669999999999987</v>
       </c>
       <c r="E86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="F86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="G86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="H86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="I86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="J86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.8829999999999991</v>
       </c>
       <c r="K86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.6329999999999991</v>
       </c>
       <c r="L86" s="15">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>8.6329999999999991</v>
       </c>
       <c r="O86" s="44">
@@ -28995,7 +28997,7 @@
         <v>6.6375080000000004</v>
       </c>
       <c r="Q86" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1.0669999999999999</v>
       </c>
       <c r="R86" s="43">
@@ -29027,7 +29029,7 @@
         <v>6.977665</v>
       </c>
       <c r="Q87" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>1.0169999999999999</v>
       </c>
       <c r="R87" s="43">
@@ -29046,39 +29048,39 @@
         <v>9.7228600849999989</v>
       </c>
       <c r="D88" s="15">
-        <f t="shared" ref="D88:L88" si="34">IF(D$23&lt;&gt;"",D80-D83-D84,"")</f>
+        <f t="shared" ref="D88:L88" si="35">IF(D$23&lt;&gt;"",D80-D83-D84,"")</f>
         <v>9.321006484999403</v>
       </c>
       <c r="E88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.0122623349994058</v>
       </c>
       <c r="F88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.7119076850000035</v>
       </c>
       <c r="G88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.4201686349994098</v>
       </c>
       <c r="H88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.1370451849994119</v>
       </c>
       <c r="I88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.8614603849994147</v>
       </c>
       <c r="J88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.5944911849994163</v>
       </c>
       <c r="K88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.5848642849994174</v>
       </c>
       <c r="L88" s="15">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.5752373849994168</v>
       </c>
       <c r="O88" s="44">
@@ -29089,7 +29091,7 @@
         <v>7.3260519999999998</v>
       </c>
       <c r="Q88" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.96699999999999986</v>
       </c>
       <c r="R88" s="43">
@@ -29108,39 +29110,39 @@
         <v>0</v>
       </c>
       <c r="D89" s="15">
-        <f t="shared" ref="D89:L89" si="35">IF(D$23&lt;&gt;"",D81-D85,"")</f>
+        <f t="shared" ref="D89:L89" si="36">IF(D$23&lt;&gt;"",D81-D85,"")</f>
         <v>0</v>
       </c>
       <c r="E89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="F89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="G89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="H89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="K89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L89" s="15">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O89" s="44">
@@ -29151,7 +29153,7 @@
         <v>7.6828779999999997</v>
       </c>
       <c r="Q89" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.71700000000000008</v>
       </c>
       <c r="R89" s="43">
@@ -29171,39 +29173,39 @@
         <v>9.7228600849999989</v>
       </c>
       <c r="D90" s="15">
-        <f t="shared" ref="D90:L90" si="36">IF(D$23&lt;&gt;"",SUM(D88:D89),"")</f>
+        <f t="shared" ref="D90:L90" si="37">IF(D$23&lt;&gt;"",SUM(D88:D89),"")</f>
         <v>9.321006484999403</v>
       </c>
       <c r="E90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>9.0122623349994058</v>
       </c>
       <c r="F90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>8.7119076850000035</v>
       </c>
       <c r="G90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>8.4201686349994098</v>
       </c>
       <c r="H90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>8.1370451849994119</v>
       </c>
       <c r="I90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>7.8614603849994147</v>
       </c>
       <c r="J90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>7.5944911849994163</v>
       </c>
       <c r="K90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>7.5848642849994174</v>
       </c>
       <c r="L90" s="15">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>7.5752373849994168</v>
       </c>
       <c r="O90" s="44">
@@ -29214,7 +29216,7 @@
         <v>9.6009879999900001</v>
       </c>
       <c r="Q90" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.63300000000000001</v>
       </c>
       <c r="R90" s="43">
@@ -29233,7 +29235,7 @@
         <v>10.857008</v>
       </c>
       <c r="Q91" s="47">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.3</v>
       </c>
       <c r="R91" s="49"/>
@@ -29254,35 +29256,35 @@
         <v>0.2</v>
       </c>
       <c r="E92" s="12">
-        <f t="shared" ref="E92:L92" si="37">IF(E$23&lt;&gt;"",D92,"")</f>
+        <f t="shared" ref="E92:L92" si="38">IF(E$23&lt;&gt;"",D92,"")</f>
         <v>0.2</v>
       </c>
       <c r="F92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="G92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="H92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="I92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="J92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="K92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="L92" s="12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
     </row>
@@ -29295,39 +29297,39 @@
         <v>7.0670000000000002</v>
       </c>
       <c r="D93" s="15">
-        <f t="shared" ref="D93:L93" si="38">IF(D$23&lt;&gt;"",SUM(D83,D92),"")</f>
+        <f t="shared" ref="D93:L93" si="39">IF(D$23&lt;&gt;"",SUM(D83,D92),"")</f>
         <v>7.0670000000000002</v>
       </c>
       <c r="E93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="F93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="G93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="H93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="I93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="J93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.9829999999999997</v>
       </c>
       <c r="K93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.7330000000000005</v>
       </c>
       <c r="L93" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>6.7330000000000005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 10-year accounting in comparison to curtailment volume. Paria flows
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE54361-76BA-462E-BE60-D4A4037A86AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC96F75-1B33-42E3-9162-0B8576035053}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="1" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
@@ -951,7 +951,7 @@
     <xf numFmtId="167" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -959,15 +959,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -981,16 +972,25 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -18695,7 +18695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -18715,20 +18715,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -18745,36 +18745,36 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="1:12" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="16"/>
@@ -18790,20 +18790,20 @@
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="62"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="59"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
@@ -19075,19 +19075,19 @@
       <c r="A23" s="29">
         <v>14</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="61"/>
     </row>
     <row r="24" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
@@ -19199,37 +19199,37 @@
       <c r="A30" s="29">
         <v>20</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="57"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="61"/>
     </row>
     <row r="31" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
         <v>21</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="63"/>
-      <c r="I31" s="63"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="64"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="63"/>
     </row>
     <row r="32" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
@@ -19306,23 +19306,33 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="59" t="s">
+      <c r="A42" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="59"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="56"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="56"/>
+      <c r="L42" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A5:L5"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
@@ -19339,16 +19349,6 @@
     <mergeCell ref="B19:L19"/>
     <mergeCell ref="B20:L20"/>
     <mergeCell ref="B21:L21"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19358,7 +19358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3356767-5983-45FB-80E4-1C5DE08E38A0}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -19420,48 +19420,48 @@
         <v>61</v>
       </c>
       <c r="B5" s="13"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="13"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -23498,48 +23498,48 @@
         <v>61</v>
       </c>
       <c r="B5" s="38"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="38"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="38"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="38"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -26496,48 +26496,48 @@
         <v>61</v>
       </c>
       <c r="B5" s="38"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="38"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="38"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="38"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
@@ -27219,7 +27219,7 @@
       <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="66">
+      <c r="B35" s="53">
         <v>7.5</v>
       </c>
       <c r="C35" s="15">
@@ -47311,10 +47311,10 @@
   <dimension ref="A1:M689"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B325" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:C676"/>
+      <selection pane="bottomRight" activeCell="A335" sqref="A335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add Powell + Mead as combined reservoir
</commit_message>
<xml_diff>
--- a/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
+++ b/InteractiveWaterBudget/InteractiveWaterBudget-PowellMead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\InteractiveWaterBudget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC96F75-1B33-42E3-9162-0B8576035053}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C865F8-F177-44C0-A020-7CF6A7914C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="1" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6640" activeTab="4" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
@@ -954,11 +954,23 @@
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -972,23 +984,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18695,7 +18695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -18715,20 +18715,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -18745,36 +18745,36 @@
       <c r="D3"/>
     </row>
     <row r="4" spans="1:12" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
     </row>
     <row r="5" spans="1:12" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
     </row>
     <row r="6" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="16"/>
@@ -18790,92 +18790,92 @@
       <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="59"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="63"/>
     </row>
     <row r="8" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
         <v>1</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29">
         <v>2</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="56"/>
     </row>
     <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
         <v>3</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="56"/>
     </row>
     <row r="11" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29">
         <v>4</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="52" t="s">
@@ -18897,91 +18897,91 @@
       <c r="A13" s="29">
         <v>5</v>
       </c>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="56"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
         <v>6</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="56"/>
     </row>
     <row r="15" spans="1:12" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29">
         <v>7</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="56"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="56"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="29">
         <v>9</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="56"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
@@ -19003,163 +19003,163 @@
       <c r="A19" s="29">
         <v>10</v>
       </c>
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="56"/>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
         <v>11</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="56"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="29">
         <v>12</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="56"/>
     </row>
     <row r="22" spans="1:12" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
         <v>13</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="55"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="56"/>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="29">
         <v>14</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="57"/>
+      <c r="L23" s="58"/>
     </row>
     <row r="24" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
         <v>15</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="55" t="s">
         <v>180</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="56"/>
     </row>
     <row r="25" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="29">
         <v>16</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="56"/>
     </row>
     <row r="26" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29">
         <v>17</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="56"/>
     </row>
     <row r="27" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="29">
         <v>18</v>
       </c>
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="56"/>
     </row>
     <row r="28" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="52" t="s">
@@ -19181,55 +19181,55 @@
       <c r="A29" s="29">
         <v>19</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="56"/>
     </row>
     <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="29">
         <v>20</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="61"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="58"/>
     </row>
     <row r="31" spans="1:12" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="29">
         <v>21</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="64" t="s">
         <v>176</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="62"/>
-      <c r="K31" s="62"/>
-      <c r="L31" s="63"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="65"/>
     </row>
     <row r="32" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
@@ -19306,33 +19306,23 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="60" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="60"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+      <c r="H42" s="60"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="60"/>
+      <c r="L42" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A5:L5"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
@@ -19349,6 +19339,16 @@
     <mergeCell ref="B19:L19"/>
     <mergeCell ref="B20:L20"/>
     <mergeCell ref="B21:L21"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19358,7 +19358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3356767-5983-45FB-80E4-1C5DE08E38A0}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -23437,7 +23439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81529C05-1E12-43A2-A554-D17F7CC4852D}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -26433,8 +26435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551E70D5-97BA-4F5D-AF13-D96C10A68BB9}">
   <dimension ref="A1:S93"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>